<commit_message>
Small addition to network_commands and deleted old file
</commit_message>
<xml_diff>
--- a/doc/raw/network_commands.xlsx
+++ b/doc/raw/network_commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bram\Stage (semester 5)\VelaLab\vela-lab\doc\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{952B6A59-CAF0-423B-9180-5DE7880BA516}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{00175E78-5376-4341-B119-AB4C5B5A2105}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7416"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Command</t>
   </si>
@@ -210,6 +210,22 @@
   </si>
   <si>
     <t>[uint8_t pkt_len] [pkttype_t pkttype] [payload]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Liberation Sans"/>
+      </rPr>
+      <t>The n in (n) behind elements of the payload indicates the size in bytes of that element</t>
+    </r>
+  </si>
+  <si>
+    <t>Keep alive message from CC2650 to gateway</t>
   </si>
 </sst>
 </file>
@@ -433,7 +449,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -468,6 +483,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Accent" xfId="1"/>
@@ -799,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD37"/>
+  <dimension ref="A1:XFD38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -819,7 +835,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -878,27 +894,27 @@
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4"/>
-      <c r="B11" s="10"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
@@ -923,205 +939,210 @@
       <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="15"/>
+      <c r="E16" s="14"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15" t="s">
+      <c r="C18" s="14"/>
+      <c r="D18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="15"/>
+      <c r="E18" s="14"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
+      <c r="C20" s="14"/>
+      <c r="D20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="15"/>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" spans="1:5" ht="45" customHeight="1">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="15"/>
+      <c r="E22" s="14"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15" t="s">
+      <c r="C24" s="14"/>
+      <c r="D24" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15" t="s">
+      <c r="C26" s="14"/>
+      <c r="D26" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="15"/>
+      <c r="E26" s="14"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15" t="s">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="15"/>
+      <c r="E30" s="14"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="15"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15" t="s">
+      <c r="C32" s="14"/>
+      <c r="D32" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="15"/>
+      <c r="E32" s="14"/>
     </row>
     <row r="34" spans="1:1" ht="15.6">
       <c r="A34" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="8"/>
-    </row>
-    <row r="36" spans="1:1" ht="15.6">
-      <c r="A36" s="1" t="s">
+    <row r="35" spans="1:1" ht="15.6">
+      <c r="A35" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.6">
+      <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:1">
+      <c r="A38" s="2" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
allign matlab/octave version with the new ipv6 IDs
</commit_message>
<xml_diff>
--- a/doc/raw/network_commands.xlsx
+++ b/doc/raw/network_commands.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bram\Stage (semester 5)\VelaLab\vela-lab\doc\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\workspaces\GIT\vela-lab\doc\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{00175E78-5376-4341-B119-AB4C5B5A2105}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7A8C07-BC0E-43FD-8AC4-09497B7FEA09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7416"/>
+    <workbookView xWindow="-4290" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
   <si>
     <t>Command</t>
   </si>
@@ -136,15 +136,6 @@
     <t>n is amount of contactdata elements in packet, 0 &lt; n &lt; 7</t>
   </si>
   <si>
-    <t xml:space="preserve"> [active_scan] [scan_interval](2) [scan_window](2) [timeout](2)
-[report_timeout](4)</t>
-  </si>
-  <si>
-    <t>Active_scan: bool to enable scanning. Scan_interval: scan interval in ms.
-Scan_window: scan window in ms. Timeout: scanning timeout in s. 
-Report_timeout: Interval of generating reports in s.</t>
-  </si>
-  <si>
     <t>nordic_turn_bt_on_low</t>
   </si>
   <si>
@@ -194,6 +185,18 @@
   </si>
   <si>
     <t>Resets the Nordic upon receiving the message</t>
+  </si>
+  <si>
+    <t>[uint8_t pkt_len] [pkttype_t pkttype] [payload]</t>
+  </si>
+  <si>
+    <t>Keep alive message from CC2650 to gateway</t>
+  </si>
+  <si>
+    <t>Active_scan: bool to enable scanning. Scan_interval: scan interval in ms. Scan_window: scan window in ms. Timeout: scanning timeout in s. Report_timeout: Interval of generating reports in s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [active_scan] [scan_interval](2) [scan_window](2) [timeout](2) [report_timeout](4)</t>
   </si>
   <si>
     <r>
@@ -201,15 +204,14 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="4" tint="-0.249977111117893"/>
-        <rFont val="Liberation Sans"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
       </rPr>
       <t>Blue messages are trickle messages that have separate counters from the other messages</t>
     </r>
-  </si>
-  <si>
-    <t>[uint8_t pkt_len] [pkttype_t pkttype] [payload]</t>
   </si>
   <si>
     <r>
@@ -217,21 +219,77 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Liberation Sans"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
       </rPr>
       <t>The n in (n) behind elements of the payload indicates the size in bytes of that element</t>
     </r>
   </si>
   <si>
-    <t>Keep alive message from CC2650 to gateway</t>
+    <t>ota_start_of_firmware</t>
+  </si>
+  <si>
+    <t>ota_more_of_firmware</t>
+  </si>
+  <si>
+    <t>ota_end_of_firmware</t>
+  </si>
+  <si>
+    <t>ota_ack</t>
+  </si>
+  <si>
+    <t>ota_reboot_node</t>
+  </si>
+  <si>
+    <t>0x0020</t>
+  </si>
+  <si>
+    <t>0x0021</t>
+  </si>
+  <si>
+    <t>0x0022</t>
+  </si>
+  <si>
+    <t>0x0023</t>
+  </si>
+  <si>
+    <t>0x0024</t>
+  </si>
+  <si>
+    <t>[first_firmware_packet]</t>
+  </si>
+  <si>
+    <t>[more_firmware_packet]</t>
+  </si>
+  <si>
+    <t>[last_firmware_packet]</t>
+  </si>
+  <si>
+    <t>node-&gt;sink direction. Sent every fimrware chunk (OTA_CHUNK_SIZE=256Bytes) received. If err_code=0 the chunk have no problems. Otherwise it should be resent</t>
+  </si>
+  <si>
+    <t>[reboot delay since the packet is received]</t>
+  </si>
+  <si>
+    <t>only the first packet of a firmware should use this. It triggers the flash erase.</t>
+  </si>
+  <si>
+    <t>only the last packet of a firmware should use this. It triggers the CRC validation.</t>
+  </si>
+  <si>
+    <t>[last_firmware_chunk_received][err_code]</t>
+  </si>
+  <si>
+    <t>reboots the node. In case an OTA has been pushed, the reboot is required to flash the new fimrware version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20">
     <font>
       <sz val="11"/>
@@ -309,37 +367,46 @@
       <name val="Liberation Sans"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Liberation Sans"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFA52A2A"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
       <b/>
-      <sz val="12"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="4" tint="-0.249977111117893"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Liberation Sans"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="9">
@@ -436,74 +503,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="18">
-    <cellStyle name="Accent" xfId="1"/>
-    <cellStyle name="Accent 1" xfId="2"/>
-    <cellStyle name="Accent 2" xfId="3"/>
-    <cellStyle name="Accent 3" xfId="4"/>
-    <cellStyle name="Bad" xfId="5"/>
-    <cellStyle name="Error" xfId="6"/>
-    <cellStyle name="Footnote" xfId="7"/>
-    <cellStyle name="Good" xfId="8"/>
-    <cellStyle name="Heading" xfId="9"/>
-    <cellStyle name="Heading 1" xfId="10"/>
-    <cellStyle name="Heading 2" xfId="11"/>
-    <cellStyle name="Hyperlink" xfId="12"/>
-    <cellStyle name="Neutral" xfId="13"/>
-    <cellStyle name="Note" xfId="14"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Status" xfId="15"/>
-    <cellStyle name="Text" xfId="16"/>
-    <cellStyle name="Warning" xfId="17"/>
+    <cellStyle name="Accent" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Bad" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Error" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Footnote" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Good" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Heading" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Heading 1" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Heading 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Hyperlink" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Neutral" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Status" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Text" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Warning" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -519,7 +568,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -814,340 +863,427 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.8984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.09765625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="57.59765625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="66.3984375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.296875" style="2" customWidth="1"/>
-    <col min="6" max="1024" width="10.69921875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="148.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.25" style="1" customWidth="1"/>
+    <col min="6" max="1024" width="10.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D9" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D10" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2" t="s">
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1">
+      <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="11" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1">
+      <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D14" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="5" t="s">
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1">
+      <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D15" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="2" t="s">
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1">
+      <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1">
+      <c r="A24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1">
+      <c r="A25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1">
+      <c r="A26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1">
+      <c r="A28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1">
+      <c r="A30" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" ht="15" customHeight="1">
+      <c r="A31" s="9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="14"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-    </row>
-    <row r="22" spans="1:5" ht="45" customHeight="1">
-      <c r="A22" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="14"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="14"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="14" t="s">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" ht="15" customHeight="1">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="14"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="14"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" s="14"/>
-    </row>
-    <row r="34" spans="1:1" ht="15.6">
-      <c r="A34" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="15.6">
-      <c r="A35" s="20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="15.6">
-      <c r="A37" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>